<commit_message>
Added late days to demo data"
</commit_message>
<xml_diff>
--- a/test-data/demo_grades.xlsx
+++ b/test-data/demo_grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurmasz/Documents/Courses/CIS371/F22/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurmasz/Documents/Code/AltGradebook/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60159985-8119-9B4B-86DC-93A03977CCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E54358-4BEC-694B-9F45-10705CDE20AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="500" windowWidth="28500" windowHeight="17600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="500" windowWidth="28500" windowHeight="17600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="125">
   <si>
     <t>Last Name</t>
   </si>
@@ -381,6 +381,36 @@
   </si>
   <si>
     <t>William</t>
+  </si>
+  <si>
+    <t>C Project</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>m|1</t>
+  </si>
+  <si>
+    <t>p|5</t>
+  </si>
+  <si>
+    <t>m|3</t>
+  </si>
+  <si>
+    <t>m|4</t>
+  </si>
+  <si>
+    <t>pm|3</t>
+  </si>
+  <si>
+    <t>m|2</t>
+  </si>
+  <si>
+    <t>p|2</t>
+  </si>
+  <si>
+    <t>pm|1</t>
   </si>
 </sst>
 </file>
@@ -1397,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1760,7 +1790,7 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="G11" t="s">
         <v>67</v>
@@ -1826,7 +1856,7 @@
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="G13" t="s">
         <v>65</v>
@@ -1925,7 +1955,7 @@
         <v>21</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="G16" t="s">
         <v>18</v>
@@ -1958,7 +1988,7 @@
         <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>123</v>
       </c>
       <c r="G17" t="s">
         <v>28</v>
@@ -2024,7 +2054,7 @@
         <v>67</v>
       </c>
       <c r="F19" t="s">
-        <v>26</v>
+        <v>124</v>
       </c>
       <c r="G19" t="s">
         <v>18</v>
@@ -2057,7 +2087,7 @@
         <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>18</v>
+        <v>122</v>
       </c>
       <c r="G20" t="s">
         <v>67</v>
@@ -2328,15 +2358,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" t="str">
         <f>info!A1</f>
         <v>Last Name</v>
@@ -2353,8 +2383,11 @@
         <f>info!E1</f>
         <v>GitHub</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A2" t="str">
         <f>info!A2</f>
         <v>lname</v>
@@ -2371,8 +2404,11 @@
         <f>info!E2</f>
         <v>github</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A3" t="str">
         <f>info!A3</f>
         <v>Bright</v>
@@ -2389,8 +2425,11 @@
         <f>info!E3</f>
         <v>brightw</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A4" t="str">
         <f>info!A4</f>
         <v>Dean</v>
@@ -2407,8 +2446,11 @@
         <f>info!E4</f>
         <v>deane</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="str">
         <f>info!A5</f>
         <v>Flowers</v>
@@ -2425,8 +2467,11 @@
         <f>info!E5</f>
         <v>flowersj</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" t="str">
         <f>info!A6</f>
         <v>Frank</v>
@@ -2443,8 +2488,11 @@
         <f>info!E6</f>
         <v>frankc</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A7" t="str">
         <f>info!A7</f>
         <v>Henry</v>
@@ -2461,8 +2509,11 @@
         <f>info!E7</f>
         <v>henryd</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" t="str">
         <f>info!A8</f>
         <v>Howel</v>
@@ -2479,8 +2530,11 @@
         <f>info!E8</f>
         <v>howelh</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" t="str">
         <f>info!A9</f>
         <v>Jacobs</v>
@@ -2497,8 +2551,11 @@
         <f>info!E9</f>
         <v>jacobsd</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" t="str">
         <f>info!A10</f>
         <v>Jackson</v>
@@ -2515,8 +2572,11 @@
         <f>info!E10</f>
         <v>jacksonr</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A11" t="str">
         <f>info!A11</f>
         <v>King</v>
@@ -2533,8 +2593,11 @@
         <f>info!E11</f>
         <v>kinga</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" t="str">
         <f>info!A12</f>
         <v>Klein</v>
@@ -2551,8 +2614,11 @@
         <f>info!E12</f>
         <v>kleinb</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A13" t="str">
         <f>info!A13</f>
         <v>Lowery</v>
@@ -2569,8 +2635,11 @@
         <f>info!E13</f>
         <v>loweryn</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A14" t="str">
         <f>info!A14</f>
         <v>Mckinney</v>
@@ -2587,8 +2656,11 @@
         <f>info!E14</f>
         <v>mckinneyl</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A15" t="str">
         <f>info!A15</f>
         <v>Mills</v>
@@ -2605,8 +2677,11 @@
         <f>info!E15</f>
         <v>millsl</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" t="str">
         <f>info!A16</f>
         <v>Morrison</v>
@@ -2623,8 +2698,11 @@
         <f>info!E16</f>
         <v>morrisonr</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A17" t="str">
         <f>info!A17</f>
         <v>Nguyen</v>
@@ -2641,8 +2719,11 @@
         <f>info!E17</f>
         <v>nguyenb</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A18" t="str">
         <f>info!A18</f>
         <v>Noraburta</v>
@@ -2659,8 +2740,11 @@
         <f>info!E18</f>
         <v>noraburtap</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A19" t="str">
         <f>info!A19</f>
         <v>Nunez</v>
@@ -2677,8 +2761,11 @@
         <f>info!E19</f>
         <v>nunezs</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A20" t="str">
         <f>info!A20</f>
         <v>Patterson</v>
@@ -2695,8 +2782,11 @@
         <f>info!E20</f>
         <v>pattersonl</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A21" t="str">
         <f>info!A21</f>
         <v>Poole</v>
@@ -2713,8 +2803,11 @@
         <f>info!E21</f>
         <v>poolem</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="str">
         <f>info!A22</f>
         <v>Phillips</v>
@@ -2731,8 +2824,11 @@
         <f>info!E22</f>
         <v>phillipsr</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="str">
         <f>info!A23</f>
         <v>Shearman</v>
@@ -2749,8 +2845,11 @@
         <f>info!E23</f>
         <v>shearmanc</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="str">
         <f>info!A24</f>
         <v>Spears</v>
@@ -2767,8 +2866,11 @@
         <f>info!E24</f>
         <v>spearsc</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="str">
         <f>info!A25</f>
         <v>Tate</v>
@@ -2785,8 +2887,11 @@
         <f>info!E25</f>
         <v>tatea</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="str">
         <f>info!A26</f>
         <v>Taylor</v>
@@ -2803,8 +2908,11 @@
         <f>info!E26</f>
         <v>taylora</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="str">
         <f>info!A27</f>
         <v>Waterson</v>
@@ -2821,8 +2929,11 @@
         <f>info!E27</f>
         <v>watersonw</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="str">
         <f>info!A28</f>
         <v>Zyer</v>
@@ -2838,6 +2949,9 @@
       <c r="D28" t="str">
         <f>info!E28</f>
         <v>zyerb</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -3763,7 +3877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91792C2-488C-3549-A3D4-732CA45379CB}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Only take highest mark from each entry
</commit_message>
<xml_diff>
--- a/test-data/demo_grades.xlsx
+++ b/test-data/demo_grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kurmasz/Documents/Code/AltGradebook/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E54358-4BEC-694B-9F45-10705CDE20AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840124AA-EE9E-6D47-BF92-7BEC79AA7D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="500" windowWidth="28500" windowHeight="17600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="128">
   <si>
     <t>Last Name</t>
   </si>
@@ -411,6 +411,15 @@
   </si>
   <si>
     <t>pm|1</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>xpm</t>
+  </si>
+  <si>
+    <t>mxx</t>
   </si>
 </sst>
 </file>
@@ -1428,7 +1437,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1853,7 +1862,7 @@
         <v>loweryn</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>127</v>
       </c>
       <c r="F13" t="s">
         <v>119</v>
@@ -1862,10 +1871,10 @@
         <v>65</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
+        <v>125</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">

</xml_diff>